<commit_message>
fine/jail info & raw info
</commit_message>
<xml_diff>
--- a/Case Details.xlsx
+++ b/Case Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Full Case Number</t>
   </si>
@@ -55,16 +55,34 @@
     <t xml:space="preserve">Disposition</t>
   </si>
   <si>
-    <t xml:space="preserve">Full Offense Details</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fine Paid?</t>
   </si>
   <si>
     <t xml:space="preserve">Fines</t>
   </si>
   <si>
-    <t xml:space="preserve">Jail Sentence</t>
+    <t xml:space="preserve">Payments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined Fees/Fines/Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jail Sentence(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentence Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Case Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Offense Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Payments Made to the Court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Register of Actions</t>
   </si>
 </sst>
 </file>
@@ -74,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,6 +114,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -114,6 +140,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -140,12 +173,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,10 +207,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,59 +222,84 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="25.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="40.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="40.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="41.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="57.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add'l patterns probation completion and setaside
</commit_message>
<xml_diff>
--- a/Case Details.xlsx
+++ b/Case Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Case Title</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sentence Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probation Terminated?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Aside?</t>
   </si>
   <si>
     <t xml:space="preserve">Raw Payments Made to the Court</t>
@@ -209,8 +215,8 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -230,8 +236,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="18.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="41.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="57.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="1" width="41.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="57.72"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,10 +304,14 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="XEY1" s="0"/>
-      <c r="XEZ1" s="0"/>
-      <c r="XFA1" s="0"/>
-      <c r="XFB1" s="0"/>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="XFA1" s="1"/>
+      <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>

</xml_diff>